<commit_message>
add mock redis, add test case MedicalExaminationRepository
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CheckedOrderDataSample.xlsx
+++ b/CloudTest/SampleData/CheckedOrderDataSample.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\emr-cloud-be(new)\emr-cloud-be\CloudTest\SampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartKarteBE\emr-cloud-be\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85DFB34-FC50-4EEC-918A-812877AFA38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE6CB93-AEC8-4780-B637-8DA4B3AE66CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{1EE0AC96-80AB-44A0-ACE0-FD2CAF1FB7F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{1EE0AC96-80AB-44A0-ACE0-FD2CAF1FB7F4}"/>
   </bookViews>
   <sheets>
     <sheet name="RAIIN_INF" sheetId="1" r:id="rId1"/>
     <sheet name="ODR_INF" sheetId="18" r:id="rId2"/>
     <sheet name="ODR_INF_DETAIL" sheetId="19" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="22" r:id="rId4"/>
+    <sheet name="TEN_MST" sheetId="22" r:id="rId4"/>
     <sheet name="PT_SANTEI_CONF" sheetId="20" r:id="rId5"/>
     <sheet name="USER_MST" sheetId="21" r:id="rId6"/>
     <sheet name="TEKIOU_BYOMEI_MST" sheetId="23" r:id="rId7"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="307">
   <si>
     <t>HP_ID</t>
   </si>
@@ -437,6 +437,522 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>NameUnitTest</t>
+  </si>
+  <si>
+    <t>KanaName1Test</t>
+  </si>
+  <si>
+    <t>KanaName2Test</t>
+  </si>
+  <si>
+    <t>ガスター散２％</t>
+  </si>
+  <si>
+    <t>ｇ</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>2325003B2029</t>
+  </si>
+  <si>
+    <t>2325003B2</t>
+  </si>
+  <si>
+    <t>2021-04-01 00:00:00.000</t>
+  </si>
+  <si>
+    <t>MASTER_SBT</t>
+  </si>
+  <si>
+    <t>RYOSYU_NAME</t>
+  </si>
+  <si>
+    <t>RECE_NAME</t>
+  </si>
+  <si>
+    <t>TEN_ID</t>
+  </si>
+  <si>
+    <t>TEN</t>
+  </si>
+  <si>
+    <t>RECE_UNIT_CD</t>
+  </si>
+  <si>
+    <t>RECE_UNIT_NAME</t>
+  </si>
+  <si>
+    <t>ODR_UNIT_NAME</t>
+  </si>
+  <si>
+    <t>CNV_UNIT_NAME</t>
+  </si>
+  <si>
+    <t>ODR_TERM_VAL</t>
+  </si>
+  <si>
+    <t>CNV_TERM_VAL</t>
+  </si>
+  <si>
+    <t>DEFAULT_VAL</t>
+  </si>
+  <si>
+    <t>KOUKI_KBN</t>
+  </si>
+  <si>
+    <t>HOKATU_KENSA</t>
+  </si>
+  <si>
+    <t>BYOMEI_KBN</t>
+  </si>
+  <si>
+    <t>IGAKUKANRI</t>
+  </si>
+  <si>
+    <t>JITUDAY_COUNT</t>
+  </si>
+  <si>
+    <t>JITUDAY</t>
+  </si>
+  <si>
+    <t>DAY_COUNT</t>
+  </si>
+  <si>
+    <t>DRUG_KANREN_KBN</t>
+  </si>
+  <si>
+    <t>KIZAMI_ID</t>
+  </si>
+  <si>
+    <t>KIZAMI_MIN</t>
+  </si>
+  <si>
+    <t>KIZAMI_MAX</t>
+  </si>
+  <si>
+    <t>KIZAMI_VAL</t>
+  </si>
+  <si>
+    <t>KIZAMI_TEN</t>
+  </si>
+  <si>
+    <t>KIZAMI_ERR</t>
+  </si>
+  <si>
+    <t>MAX_COUNT</t>
+  </si>
+  <si>
+    <t>MAX_COUNT_ERR</t>
+  </si>
+  <si>
+    <t>TYU_CD</t>
+  </si>
+  <si>
+    <t>TYU_SEQ</t>
+  </si>
+  <si>
+    <t>TUSOKU_AGE</t>
+  </si>
+  <si>
+    <t>MIN_AGE</t>
+  </si>
+  <si>
+    <t>MAX_AGE</t>
+  </si>
+  <si>
+    <t>TIME_KASAN_KBN</t>
+  </si>
+  <si>
+    <t>FUTEKI_KBN</t>
+  </si>
+  <si>
+    <t>FUTEKI_SISETU_KBN</t>
+  </si>
+  <si>
+    <t>SYOTI_NYUYOJI_KBN</t>
+  </si>
+  <si>
+    <t>LOW_WEIGHT_KBN</t>
+  </si>
+  <si>
+    <t>HANDAN_KBN</t>
+  </si>
+  <si>
+    <t>HANDAN_GRP_KBN</t>
+  </si>
+  <si>
+    <t>TEIGEN_KBN</t>
+  </si>
+  <si>
+    <t>SEKITUI_KBN</t>
+  </si>
+  <si>
+    <t>KEIBU_KBN</t>
+  </si>
+  <si>
+    <t>AUTO_HOUGOU_KBN</t>
+  </si>
+  <si>
+    <t>GAIRAI_KANRI_KBN</t>
+  </si>
+  <si>
+    <t>TUSOKU_TARGET_KBN</t>
+  </si>
+  <si>
+    <t>HOKATU_KBN</t>
+  </si>
+  <si>
+    <t>TYOONPA_NAISI_KBN</t>
+  </si>
+  <si>
+    <t>AUTO_FUNGO_KBN</t>
+  </si>
+  <si>
+    <t>TYOONPA_GYOKO_KBN</t>
+  </si>
+  <si>
+    <t>GAZO_KASAN</t>
+  </si>
+  <si>
+    <t>KANSATU_KBN</t>
+  </si>
+  <si>
+    <t>MASUI_KBN</t>
+  </si>
+  <si>
+    <t>FUKUBIKU_NAISI_KASAN</t>
+  </si>
+  <si>
+    <t>FUKUBIKU_KOTUNAN_KASAN</t>
+  </si>
+  <si>
+    <t>MASUI_KASAN</t>
+  </si>
+  <si>
+    <t>MONITER_KASAN</t>
+  </si>
+  <si>
+    <t>TOKETU_KASAN</t>
+  </si>
+  <si>
+    <t>TEN_KBN_NO</t>
+  </si>
+  <si>
+    <t>SHORTSTAY_OPE</t>
+  </si>
+  <si>
+    <t>BUI_KBN</t>
+  </si>
+  <si>
+    <t>SISETUCD1</t>
+  </si>
+  <si>
+    <t>SISETUCD2</t>
+  </si>
+  <si>
+    <t>SISETUCD3</t>
+  </si>
+  <si>
+    <t>SISETUCD4</t>
+  </si>
+  <si>
+    <t>SISETUCD5</t>
+  </si>
+  <si>
+    <t>SISETUCD6</t>
+  </si>
+  <si>
+    <t>SISETUCD7</t>
+  </si>
+  <si>
+    <t>SISETUCD8</t>
+  </si>
+  <si>
+    <t>SISETUCD9</t>
+  </si>
+  <si>
+    <t>SISETUCD10</t>
+  </si>
+  <si>
+    <t>AGEKASAN_MIN1</t>
+  </si>
+  <si>
+    <t>AGEKASAN_MAX1</t>
+  </si>
+  <si>
+    <t>AGEKASAN_CD1</t>
+  </si>
+  <si>
+    <t>AGEKASAN_MIN2</t>
+  </si>
+  <si>
+    <t>AGEKASAN_MAX2</t>
+  </si>
+  <si>
+    <t>AGEKASAN_CD2</t>
+  </si>
+  <si>
+    <t>AGEKASAN_MIN3</t>
+  </si>
+  <si>
+    <t>AGEKASAN_MAX3</t>
+  </si>
+  <si>
+    <t>AGEKASAN_CD3</t>
+  </si>
+  <si>
+    <t>AGEKASAN_MIN4</t>
+  </si>
+  <si>
+    <t>AGEKASAN_MAX4</t>
+  </si>
+  <si>
+    <t>AGEKASAN_CD4</t>
+  </si>
+  <si>
+    <t>KENSA_CMT</t>
+  </si>
+  <si>
+    <t>MADOKU_KBN</t>
+  </si>
+  <si>
+    <t>SINKEI_KBN</t>
+  </si>
+  <si>
+    <t>SEIBUTU_KBN</t>
+  </si>
+  <si>
+    <t>ZOUEI_KBN</t>
+  </si>
+  <si>
+    <t>ZAI_KBN</t>
+  </si>
+  <si>
+    <t>CAPACITY</t>
+  </si>
+  <si>
+    <t>TOKUZAI_AGE_KBN</t>
+  </si>
+  <si>
+    <t>SANSO_KBN</t>
+  </si>
+  <si>
+    <t>TOKUZAI_SBT</t>
+  </si>
+  <si>
+    <t>MAX_PRICE</t>
+  </si>
+  <si>
+    <t>MAX_TEN</t>
+  </si>
+  <si>
+    <t>SYUKEI_SAKI</t>
+  </si>
+  <si>
+    <t>CD_KBN</t>
+  </si>
+  <si>
+    <t>CD_SYO</t>
+  </si>
+  <si>
+    <t>CD_BU</t>
+  </si>
+  <si>
+    <t>CD_KBNNO</t>
+  </si>
+  <si>
+    <t>CD_EDANO</t>
+  </si>
+  <si>
+    <t>CD_KOUNO</t>
+  </si>
+  <si>
+    <t>KOKUJI_KBN</t>
+  </si>
+  <si>
+    <t>KOKUJI_SYO</t>
+  </si>
+  <si>
+    <t>KOKUJI_BU</t>
+  </si>
+  <si>
+    <t>KOKUJI_KBN_NO</t>
+  </si>
+  <si>
+    <t>KOKUJI_EDA_NO</t>
+  </si>
+  <si>
+    <t>KOKUJI_KOU_NO</t>
+  </si>
+  <si>
+    <t>KOHYO_JUN</t>
+  </si>
+  <si>
+    <t>YJ_CD</t>
+  </si>
+  <si>
+    <t>YAKKA_CD</t>
+  </si>
+  <si>
+    <t>SYUSAI_SBT</t>
+  </si>
+  <si>
+    <t>SYOHIN_KANREN</t>
+  </si>
+  <si>
+    <t>KEIKA_DATE</t>
+  </si>
+  <si>
+    <t>ROUSAI_KBN</t>
+  </si>
+  <si>
+    <t>SISI_KBN</t>
+  </si>
+  <si>
+    <t>SHOT_CNT</t>
+  </si>
+  <si>
+    <t>IS_NOSEARCH</t>
+  </si>
+  <si>
+    <t>IS_NODSP_PAPER_RECE</t>
+  </si>
+  <si>
+    <t>IS_NODSP_RYOSYU</t>
+  </si>
+  <si>
+    <t>IS_NODSP_KARTE</t>
+  </si>
+  <si>
+    <t>JIHI_SBT</t>
+  </si>
+  <si>
+    <t>KAZEI_KBN</t>
+  </si>
+  <si>
+    <t>IPN_NAME_CD</t>
+  </si>
+  <si>
+    <t>FUKUYO_RISE</t>
+  </si>
+  <si>
+    <t>FUKUYO_MORNING</t>
+  </si>
+  <si>
+    <t>FUKUYO_DAYTIME</t>
+  </si>
+  <si>
+    <t>FUKUYO_NIGHT</t>
+  </si>
+  <si>
+    <t>FUKUYO_SLEEP</t>
+  </si>
+  <si>
+    <t>SURYO_ROUNDUP_KBN</t>
+  </si>
+  <si>
+    <t>KOUSEISIN_KBN</t>
+  </si>
+  <si>
+    <t>SANTEI_ITEM_CD</t>
+  </si>
+  <si>
+    <t>SANTEIGAI_KBN</t>
+  </si>
+  <si>
+    <t>KENSA_ITEM_CD</t>
+  </si>
+  <si>
+    <t>KENSA_ITEM_SEQ_NO</t>
+  </si>
+  <si>
+    <t>RENKEI_CD2</t>
+  </si>
+  <si>
+    <t>SAIKETU_KBN</t>
+  </si>
+  <si>
+    <t>CMT_KBN</t>
+  </si>
+  <si>
+    <t>CMT_COL1</t>
+  </si>
+  <si>
+    <t>CMT_COL_KETA1</t>
+  </si>
+  <si>
+    <t>CMT_COL2</t>
+  </si>
+  <si>
+    <t>CMT_COL_KETA2</t>
+  </si>
+  <si>
+    <t>CMT_COL3</t>
+  </si>
+  <si>
+    <t>CMT_COL_KETA3</t>
+  </si>
+  <si>
+    <t>CMT_COL4</t>
+  </si>
+  <si>
+    <t>CMT_COL_KETA4</t>
+  </si>
+  <si>
+    <t>SELECT_CMT_ID</t>
+  </si>
+  <si>
+    <t>CHUSYA_DRUG_SBT</t>
+  </si>
+  <si>
+    <t>KENSA_FUKUSU_SANTEI</t>
+  </si>
+  <si>
+    <t>AGE_CHECK</t>
+  </si>
+  <si>
+    <t>KOKUJI_BETUNO</t>
+  </si>
+  <si>
+    <t>KOKUJI_KBNNO</t>
+  </si>
+  <si>
+    <t>CMT_SBT</t>
+  </si>
+  <si>
+    <t>IS_NODSP_YAKUTAI</t>
+  </si>
+  <si>
+    <t>ZAIKEI_POINT</t>
+  </si>
+  <si>
+    <t>KENSA_LABEL</t>
+  </si>
+  <si>
+    <t>GAIRAI_KANSEN</t>
+  </si>
+  <si>
+    <t>JIBI_AGE_KASAN</t>
+  </si>
+  <si>
+    <t>JIBI_SYONIKOKIN</t>
+  </si>
+  <si>
+    <t>Y90298</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Y90299</t>
   </si>
 </sst>
 </file>
@@ -796,33 +1312,33 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="28.5546875" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.88671875" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" customWidth="1"/>
     <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" customWidth="1"/>
-    <col min="22" max="22" width="12.140625" customWidth="1"/>
+    <col min="21" max="21" width="13.109375" customWidth="1"/>
+    <col min="22" max="22" width="12.109375" customWidth="1"/>
     <col min="24" max="24" width="12" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" customWidth="1"/>
-    <col min="28" max="28" width="13.140625" customWidth="1"/>
-    <col min="32" max="32" width="15.28515625" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.44140625" customWidth="1"/>
+    <col min="28" max="28" width="13.109375" customWidth="1"/>
+    <col min="32" max="32" width="15.33203125" customWidth="1"/>
+    <col min="33" max="33" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -920,7 +1436,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1006,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1105,32 +1621,32 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="11.44140625" customWidth="1"/>
     <col min="18" max="18" width="13" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" customWidth="1"/>
+    <col min="19" max="19" width="11.88671875" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="13.109375" customWidth="1"/>
     <col min="22" max="22" width="14" customWidth="1"/>
-    <col min="23" max="23" width="20.28515625" customWidth="1"/>
+    <col min="23" max="23" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1204,7 +1720,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1285,19 +1801,19 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="54.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="54.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="10" max="10" width="28.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1401,7 +1917,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1482,12 +1998,1559 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9146CE-ED57-41C2-9C61-24C07C4EF6D9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:GG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="CX1" workbookViewId="0">
+      <selection activeCell="DH8" sqref="DH8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="116" max="116" width="11.77734375" customWidth="1"/>
+    <col min="117" max="117" width="10.77734375" customWidth="1"/>
+    <col min="119" max="119" width="11.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:189" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" t="s">
+        <v>146</v>
+      </c>
+      <c r="P1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>148</v>
+      </c>
+      <c r="R1" t="s">
+        <v>149</v>
+      </c>
+      <c r="S1" t="s">
+        <v>150</v>
+      </c>
+      <c r="T1" t="s">
+        <v>151</v>
+      </c>
+      <c r="U1" t="s">
+        <v>152</v>
+      </c>
+      <c r="V1" t="s">
+        <v>153</v>
+      </c>
+      <c r="W1" t="s">
+        <v>154</v>
+      </c>
+      <c r="X1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>180</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>182</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>183</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>184</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>185</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>186</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>187</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>188</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>190</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>193</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>195</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>196</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>198</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>199</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>200</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>201</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>202</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>204</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>205</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>206</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>207</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>208</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>209</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>210</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>211</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>212</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>213</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>214</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>215</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>216</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>217</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>218</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>219</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>220</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>221</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>222</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>223</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>224</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>225</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>226</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>227</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>228</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>229</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>230</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>231</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>232</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>233</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>234</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>37</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>235</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>236</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>237</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>238</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>239</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>240</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>241</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>242</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>243</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>244</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>245</v>
+      </c>
+      <c r="DN1" t="s">
+        <v>246</v>
+      </c>
+      <c r="DO1" t="s">
+        <v>247</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>248</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>249</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>250</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>251</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>252</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>38</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>39</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>253</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>254</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>255</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>256</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>257</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>123</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>124</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>258</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>259</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>260</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>261</v>
+      </c>
+      <c r="EH1" t="s">
+        <v>262</v>
+      </c>
+      <c r="EI1" t="s">
+        <v>263</v>
+      </c>
+      <c r="EJ1" t="s">
+        <v>40</v>
+      </c>
+      <c r="EK1" t="s">
+        <v>264</v>
+      </c>
+      <c r="EL1" t="s">
+        <v>265</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>266</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>267</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>41</v>
+      </c>
+      <c r="EP1" t="s">
+        <v>268</v>
+      </c>
+      <c r="EQ1" t="s">
+        <v>269</v>
+      </c>
+      <c r="ER1" t="s">
+        <v>270</v>
+      </c>
+      <c r="ES1" t="s">
+        <v>271</v>
+      </c>
+      <c r="ET1" t="s">
+        <v>272</v>
+      </c>
+      <c r="EU1" t="s">
+        <v>273</v>
+      </c>
+      <c r="EV1" t="s">
+        <v>274</v>
+      </c>
+      <c r="EW1" t="s">
+        <v>275</v>
+      </c>
+      <c r="EX1" t="s">
+        <v>276</v>
+      </c>
+      <c r="EY1" t="s">
+        <v>277</v>
+      </c>
+      <c r="EZ1" t="s">
+        <v>278</v>
+      </c>
+      <c r="FA1" t="s">
+        <v>279</v>
+      </c>
+      <c r="FB1" t="s">
+        <v>92</v>
+      </c>
+      <c r="FC1" t="s">
+        <v>280</v>
+      </c>
+      <c r="FD1" t="s">
+        <v>281</v>
+      </c>
+      <c r="FE1" t="s">
+        <v>282</v>
+      </c>
+      <c r="FF1" t="s">
+        <v>283</v>
+      </c>
+      <c r="FG1" t="s">
+        <v>284</v>
+      </c>
+      <c r="FH1" t="s">
+        <v>285</v>
+      </c>
+      <c r="FI1" t="s">
+        <v>286</v>
+      </c>
+      <c r="FJ1" t="s">
+        <v>287</v>
+      </c>
+      <c r="FK1" t="s">
+        <v>288</v>
+      </c>
+      <c r="FL1" t="s">
+        <v>289</v>
+      </c>
+      <c r="FM1" t="s">
+        <v>290</v>
+      </c>
+      <c r="FN1" t="s">
+        <v>291</v>
+      </c>
+      <c r="FO1" t="s">
+        <v>23</v>
+      </c>
+      <c r="FP1" t="s">
+        <v>24</v>
+      </c>
+      <c r="FQ1" t="s">
+        <v>25</v>
+      </c>
+      <c r="FR1" t="s">
+        <v>26</v>
+      </c>
+      <c r="FS1" t="s">
+        <v>27</v>
+      </c>
+      <c r="FT1" t="s">
+        <v>28</v>
+      </c>
+      <c r="FU1" t="s">
+        <v>292</v>
+      </c>
+      <c r="FV1" t="s">
+        <v>293</v>
+      </c>
+      <c r="FW1" t="s">
+        <v>294</v>
+      </c>
+      <c r="FX1" t="s">
+        <v>295</v>
+      </c>
+      <c r="FY1" t="s">
+        <v>296</v>
+      </c>
+      <c r="FZ1" t="s">
+        <v>297</v>
+      </c>
+      <c r="GA1" t="s">
+        <v>298</v>
+      </c>
+      <c r="GB1" t="s">
+        <v>299</v>
+      </c>
+      <c r="GC1" t="s">
+        <v>300</v>
+      </c>
+      <c r="GD1" t="s">
+        <v>301</v>
+      </c>
+      <c r="GE1" t="s">
+        <v>302</v>
+      </c>
+      <c r="GF1" t="s">
+        <v>303</v>
+      </c>
+      <c r="GG1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:189" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>99999999</v>
+      </c>
+      <c r="E2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" t="s">
+        <v>138</v>
+      </c>
+      <c r="P2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>12</v>
+      </c>
+      <c r="S2">
+        <v>33</v>
+      </c>
+      <c r="T2" t="s">
+        <v>140</v>
+      </c>
+      <c r="U2" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BF2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+      <c r="BH2">
+        <v>0</v>
+      </c>
+      <c r="BI2">
+        <v>0</v>
+      </c>
+      <c r="BJ2">
+        <v>0</v>
+      </c>
+      <c r="BK2">
+        <v>0</v>
+      </c>
+      <c r="BL2">
+        <v>0</v>
+      </c>
+      <c r="BM2">
+        <v>0</v>
+      </c>
+      <c r="BN2">
+        <v>0</v>
+      </c>
+      <c r="BO2">
+        <v>0</v>
+      </c>
+      <c r="BP2">
+        <v>0</v>
+      </c>
+      <c r="BQ2">
+        <v>0</v>
+      </c>
+      <c r="BR2">
+        <v>0</v>
+      </c>
+      <c r="BS2">
+        <v>0</v>
+      </c>
+      <c r="BT2">
+        <v>0</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
+      <c r="BW2">
+        <v>0</v>
+      </c>
+      <c r="BX2">
+        <v>0</v>
+      </c>
+      <c r="BY2">
+        <v>0</v>
+      </c>
+      <c r="BZ2">
+        <v>0</v>
+      </c>
+      <c r="CA2">
+        <v>0</v>
+      </c>
+      <c r="CB2">
+        <v>0</v>
+      </c>
+      <c r="CC2">
+        <v>0</v>
+      </c>
+      <c r="CD2">
+        <v>0</v>
+      </c>
+      <c r="CE2">
+        <v>0</v>
+      </c>
+      <c r="CF2">
+        <v>0</v>
+      </c>
+      <c r="CG2">
+        <v>0</v>
+      </c>
+      <c r="CT2">
+        <v>0</v>
+      </c>
+      <c r="CU2">
+        <v>0</v>
+      </c>
+      <c r="CV2">
+        <v>0</v>
+      </c>
+      <c r="CW2">
+        <v>0</v>
+      </c>
+      <c r="CX2">
+        <v>0</v>
+      </c>
+      <c r="CY2">
+        <v>1</v>
+      </c>
+      <c r="CZ2">
+        <v>1</v>
+      </c>
+      <c r="DA2">
+        <v>0</v>
+      </c>
+      <c r="DB2">
+        <v>2</v>
+      </c>
+      <c r="DC2">
+        <v>0</v>
+      </c>
+      <c r="DD2">
+        <v>0</v>
+      </c>
+      <c r="DE2">
+        <v>0</v>
+      </c>
+      <c r="DF2">
+        <v>0</v>
+      </c>
+      <c r="DG2">
+        <v>0</v>
+      </c>
+      <c r="DH2">
+        <v>0</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>305</v>
+      </c>
+      <c r="DJ2">
+        <v>0</v>
+      </c>
+      <c r="DK2">
+        <v>0</v>
+      </c>
+      <c r="DL2">
+        <v>0</v>
+      </c>
+      <c r="DM2">
+        <v>0</v>
+      </c>
+      <c r="DN2">
+        <v>0</v>
+      </c>
+      <c r="DP2">
+        <v>0</v>
+      </c>
+      <c r="DQ2">
+        <v>0</v>
+      </c>
+      <c r="DR2">
+        <v>0</v>
+      </c>
+      <c r="DS2">
+        <v>0</v>
+      </c>
+      <c r="DT2">
+        <v>0</v>
+      </c>
+      <c r="DU2">
+        <v>0</v>
+      </c>
+      <c r="DV2">
+        <v>1</v>
+      </c>
+      <c r="DW2">
+        <v>4923</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>142</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>142</v>
+      </c>
+      <c r="DZ2">
+        <v>1</v>
+      </c>
+      <c r="EA2">
+        <v>0</v>
+      </c>
+      <c r="EB2">
+        <v>20210401</v>
+      </c>
+      <c r="EC2">
+        <v>99999999</v>
+      </c>
+      <c r="ED2">
+        <v>0</v>
+      </c>
+      <c r="EE2">
+        <v>0</v>
+      </c>
+      <c r="EF2">
+        <v>0</v>
+      </c>
+      <c r="EG2">
+        <v>0</v>
+      </c>
+      <c r="EH2">
+        <v>0</v>
+      </c>
+      <c r="EI2">
+        <v>0</v>
+      </c>
+      <c r="EJ2">
+        <v>0</v>
+      </c>
+      <c r="EK2">
+        <v>0</v>
+      </c>
+      <c r="EL2">
+        <v>0</v>
+      </c>
+      <c r="EM2">
+        <v>0</v>
+      </c>
+      <c r="EN2">
+        <v>0</v>
+      </c>
+      <c r="EO2">
+        <v>0</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>143</v>
+      </c>
+      <c r="EQ2">
+        <v>0</v>
+      </c>
+      <c r="ER2">
+        <v>0</v>
+      </c>
+      <c r="ES2">
+        <v>0</v>
+      </c>
+      <c r="ET2">
+        <v>0</v>
+      </c>
+      <c r="EU2">
+        <v>0</v>
+      </c>
+      <c r="EV2">
+        <v>0</v>
+      </c>
+      <c r="EW2">
+        <v>0</v>
+      </c>
+      <c r="EX2">
+        <v>61040607912</v>
+      </c>
+      <c r="EY2">
+        <v>0</v>
+      </c>
+      <c r="FA2">
+        <v>0</v>
+      </c>
+      <c r="FD2">
+        <v>0</v>
+      </c>
+      <c r="FE2">
+        <v>0</v>
+      </c>
+      <c r="FF2">
+        <v>0</v>
+      </c>
+      <c r="FG2">
+        <v>0</v>
+      </c>
+      <c r="FH2">
+        <v>0</v>
+      </c>
+      <c r="FI2">
+        <v>0</v>
+      </c>
+      <c r="FJ2">
+        <v>0</v>
+      </c>
+      <c r="FK2">
+        <v>0</v>
+      </c>
+      <c r="FL2">
+        <v>0</v>
+      </c>
+      <c r="FM2">
+        <v>0</v>
+      </c>
+      <c r="FN2">
+        <v>0</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>144</v>
+      </c>
+      <c r="FP2">
+        <v>99909</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>144</v>
+      </c>
+      <c r="FS2">
+        <v>99909</v>
+      </c>
+      <c r="FU2">
+        <v>0</v>
+      </c>
+      <c r="FV2">
+        <v>0</v>
+      </c>
+      <c r="FW2">
+        <v>0</v>
+      </c>
+      <c r="FX2">
+        <v>0</v>
+      </c>
+      <c r="FY2">
+        <v>0</v>
+      </c>
+      <c r="FZ2">
+        <v>0</v>
+      </c>
+      <c r="GA2">
+        <v>0</v>
+      </c>
+      <c r="GB2" t="s">
+        <v>42</v>
+      </c>
+      <c r="GC2">
+        <v>0</v>
+      </c>
+      <c r="GD2">
+        <v>0</v>
+      </c>
+      <c r="GE2">
+        <v>0</v>
+      </c>
+      <c r="GF2">
+        <v>0</v>
+      </c>
+      <c r="GG2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:189" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>99999999</v>
+      </c>
+      <c r="E3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" t="s">
+        <v>138</v>
+      </c>
+      <c r="P3" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>12</v>
+      </c>
+      <c r="S3">
+        <v>33</v>
+      </c>
+      <c r="T3" t="s">
+        <v>140</v>
+      </c>
+      <c r="U3" t="s">
+        <v>140</v>
+      </c>
+      <c r="W3" t="s">
+        <v>42</v>
+      </c>
+      <c r="X3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="AZ3">
+        <v>0</v>
+      </c>
+      <c r="BA3">
+        <v>0</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3">
+        <v>0</v>
+      </c>
+      <c r="BD3">
+        <v>0</v>
+      </c>
+      <c r="BE3">
+        <v>0</v>
+      </c>
+      <c r="BF3">
+        <v>0</v>
+      </c>
+      <c r="BG3">
+        <v>0</v>
+      </c>
+      <c r="BH3">
+        <v>0</v>
+      </c>
+      <c r="BI3">
+        <v>0</v>
+      </c>
+      <c r="BJ3">
+        <v>0</v>
+      </c>
+      <c r="BK3">
+        <v>0</v>
+      </c>
+      <c r="BL3">
+        <v>0</v>
+      </c>
+      <c r="BM3">
+        <v>0</v>
+      </c>
+      <c r="BN3">
+        <v>0</v>
+      </c>
+      <c r="BO3">
+        <v>0</v>
+      </c>
+      <c r="BP3">
+        <v>0</v>
+      </c>
+      <c r="BQ3">
+        <v>0</v>
+      </c>
+      <c r="BR3">
+        <v>0</v>
+      </c>
+      <c r="BS3">
+        <v>0</v>
+      </c>
+      <c r="BT3">
+        <v>0</v>
+      </c>
+      <c r="BV3">
+        <v>0</v>
+      </c>
+      <c r="BW3">
+        <v>0</v>
+      </c>
+      <c r="BX3">
+        <v>0</v>
+      </c>
+      <c r="BY3">
+        <v>0</v>
+      </c>
+      <c r="BZ3">
+        <v>0</v>
+      </c>
+      <c r="CA3">
+        <v>0</v>
+      </c>
+      <c r="CB3">
+        <v>0</v>
+      </c>
+      <c r="CC3">
+        <v>0</v>
+      </c>
+      <c r="CD3">
+        <v>0</v>
+      </c>
+      <c r="CE3">
+        <v>0</v>
+      </c>
+      <c r="CF3">
+        <v>0</v>
+      </c>
+      <c r="CG3">
+        <v>0</v>
+      </c>
+      <c r="CT3">
+        <v>0</v>
+      </c>
+      <c r="CU3">
+        <v>0</v>
+      </c>
+      <c r="CV3">
+        <v>0</v>
+      </c>
+      <c r="CW3">
+        <v>0</v>
+      </c>
+      <c r="CX3">
+        <v>0</v>
+      </c>
+      <c r="CY3">
+        <v>1</v>
+      </c>
+      <c r="CZ3">
+        <v>1</v>
+      </c>
+      <c r="DA3">
+        <v>0</v>
+      </c>
+      <c r="DB3">
+        <v>2</v>
+      </c>
+      <c r="DC3">
+        <v>0</v>
+      </c>
+      <c r="DD3">
+        <v>0</v>
+      </c>
+      <c r="DE3">
+        <v>0</v>
+      </c>
+      <c r="DF3">
+        <v>0</v>
+      </c>
+      <c r="DG3">
+        <v>0</v>
+      </c>
+      <c r="DH3">
+        <v>0</v>
+      </c>
+      <c r="DI3" t="s">
+        <v>305</v>
+      </c>
+      <c r="DJ3">
+        <v>0</v>
+      </c>
+      <c r="DK3">
+        <v>0</v>
+      </c>
+      <c r="DL3">
+        <v>1</v>
+      </c>
+      <c r="DM3">
+        <v>0</v>
+      </c>
+      <c r="DN3">
+        <v>0</v>
+      </c>
+      <c r="DP3">
+        <v>0</v>
+      </c>
+      <c r="DQ3">
+        <v>0</v>
+      </c>
+      <c r="DR3">
+        <v>0</v>
+      </c>
+      <c r="DS3">
+        <v>0</v>
+      </c>
+      <c r="DT3">
+        <v>0</v>
+      </c>
+      <c r="DU3">
+        <v>0</v>
+      </c>
+      <c r="DV3">
+        <v>1</v>
+      </c>
+      <c r="DW3">
+        <v>4923</v>
+      </c>
+      <c r="DX3" t="s">
+        <v>142</v>
+      </c>
+      <c r="DY3" t="s">
+        <v>142</v>
+      </c>
+      <c r="DZ3">
+        <v>1</v>
+      </c>
+      <c r="EA3">
+        <v>0</v>
+      </c>
+      <c r="EB3">
+        <v>20210401</v>
+      </c>
+      <c r="EC3">
+        <v>99999999</v>
+      </c>
+      <c r="ED3">
+        <v>0</v>
+      </c>
+      <c r="EE3">
+        <v>0</v>
+      </c>
+      <c r="EF3">
+        <v>0</v>
+      </c>
+      <c r="EG3">
+        <v>0</v>
+      </c>
+      <c r="EH3">
+        <v>0</v>
+      </c>
+      <c r="EI3">
+        <v>0</v>
+      </c>
+      <c r="EJ3">
+        <v>0</v>
+      </c>
+      <c r="EK3">
+        <v>0</v>
+      </c>
+      <c r="EL3">
+        <v>0</v>
+      </c>
+      <c r="EM3">
+        <v>0</v>
+      </c>
+      <c r="EN3">
+        <v>0</v>
+      </c>
+      <c r="EO3">
+        <v>0</v>
+      </c>
+      <c r="EP3" t="s">
+        <v>143</v>
+      </c>
+      <c r="EQ3">
+        <v>0</v>
+      </c>
+      <c r="ER3">
+        <v>0</v>
+      </c>
+      <c r="ES3">
+        <v>0</v>
+      </c>
+      <c r="ET3">
+        <v>0</v>
+      </c>
+      <c r="EU3">
+        <v>0</v>
+      </c>
+      <c r="EV3">
+        <v>0</v>
+      </c>
+      <c r="EW3">
+        <v>0</v>
+      </c>
+      <c r="EX3">
+        <v>61040607912</v>
+      </c>
+      <c r="EY3">
+        <v>0</v>
+      </c>
+      <c r="FA3">
+        <v>0</v>
+      </c>
+      <c r="FD3">
+        <v>0</v>
+      </c>
+      <c r="FE3">
+        <v>0</v>
+      </c>
+      <c r="FF3">
+        <v>0</v>
+      </c>
+      <c r="FG3">
+        <v>0</v>
+      </c>
+      <c r="FH3">
+        <v>0</v>
+      </c>
+      <c r="FI3">
+        <v>0</v>
+      </c>
+      <c r="FJ3">
+        <v>0</v>
+      </c>
+      <c r="FK3">
+        <v>0</v>
+      </c>
+      <c r="FL3">
+        <v>0</v>
+      </c>
+      <c r="FM3">
+        <v>0</v>
+      </c>
+      <c r="FN3">
+        <v>0</v>
+      </c>
+      <c r="FO3" t="s">
+        <v>144</v>
+      </c>
+      <c r="FP3">
+        <v>99909</v>
+      </c>
+      <c r="FR3" t="s">
+        <v>144</v>
+      </c>
+      <c r="FS3">
+        <v>99909</v>
+      </c>
+      <c r="FU3">
+        <v>0</v>
+      </c>
+      <c r="FV3">
+        <v>0</v>
+      </c>
+      <c r="FW3">
+        <v>0</v>
+      </c>
+      <c r="FX3">
+        <v>0</v>
+      </c>
+      <c r="FY3">
+        <v>0</v>
+      </c>
+      <c r="FZ3">
+        <v>0</v>
+      </c>
+      <c r="GA3">
+        <v>0</v>
+      </c>
+      <c r="GB3" t="s">
+        <v>42</v>
+      </c>
+      <c r="GC3">
+        <v>0</v>
+      </c>
+      <c r="GD3">
+        <v>0</v>
+      </c>
+      <c r="GE3">
+        <v>0</v>
+      </c>
+      <c r="GF3">
+        <v>0</v>
+      </c>
+      <c r="GG3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1500,26 +3563,26 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" customWidth="1"/>
-    <col min="16" max="16" width="18.5703125" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="18.5546875" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.109375" customWidth="1"/>
+    <col min="16" max="16" width="18.5546875" customWidth="1"/>
+    <col min="17" max="17" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +3632,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1613,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1670,9 +3733,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1746,7 +3809,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1824,24 +3887,24 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
+    <col min="11" max="12" width="15.88671875" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1888,7 +3951,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1938,47 +4001,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9830985-1F87-4A2C-BCAE-09A96FE9D3D2}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" customWidth="1"/>
+    <col min="14" max="14" width="16.88671875" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
     <col min="16" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" customWidth="1"/>
-    <col min="20" max="20" width="18.42578125" customWidth="1"/>
-    <col min="21" max="21" width="20.85546875" customWidth="1"/>
-    <col min="22" max="22" width="18.85546875" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" customWidth="1"/>
-    <col min="26" max="26" width="14.28515625" customWidth="1"/>
-    <col min="27" max="27" width="14.140625" customWidth="1"/>
-    <col min="28" max="28" width="14.5703125" customWidth="1"/>
+    <col min="17" max="17" width="18.44140625" customWidth="1"/>
+    <col min="18" max="18" width="17.88671875" customWidth="1"/>
+    <col min="19" max="19" width="17.5546875" customWidth="1"/>
+    <col min="20" max="20" width="18.44140625" customWidth="1"/>
+    <col min="21" max="21" width="20.88671875" customWidth="1"/>
+    <col min="22" max="22" width="18.88671875" customWidth="1"/>
+    <col min="25" max="25" width="15.88671875" customWidth="1"/>
+    <col min="26" max="26" width="14.33203125" customWidth="1"/>
+    <col min="27" max="27" width="14.109375" customWidth="1"/>
+    <col min="28" max="28" width="14.5546875" customWidth="1"/>
     <col min="29" max="29" width="16" customWidth="1"/>
-    <col min="30" max="30" width="17.85546875" customWidth="1"/>
-    <col min="31" max="31" width="22.85546875" customWidth="1"/>
-    <col min="32" max="32" width="16.7109375" customWidth="1"/>
-    <col min="33" max="33" width="15.140625" customWidth="1"/>
-    <col min="34" max="34" width="17.85546875" customWidth="1"/>
+    <col min="30" max="30" width="17.88671875" customWidth="1"/>
+    <col min="31" max="31" width="22.88671875" customWidth="1"/>
+    <col min="32" max="32" width="16.6640625" customWidth="1"/>
+    <col min="33" max="33" width="15.109375" customWidth="1"/>
+    <col min="34" max="34" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2082,7 +4145,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
add test case TrialIryoJyohoKibanCalculation
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CheckedOrderDataSample.xlsx
+++ b/CloudTest/SampleData/CheckedOrderDataSample.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartKarteBE\emr-cloud-be\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE6CB93-AEC8-4780-B637-8DA4B3AE66CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E53E226-90B0-4A7C-A4E6-B2AAB1E81666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{1EE0AC96-80AB-44A0-ACE0-FD2CAF1FB7F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{1EE0AC96-80AB-44A0-ACE0-FD2CAF1FB7F4}"/>
   </bookViews>
   <sheets>
     <sheet name="RAIIN_INF" sheetId="1" r:id="rId1"/>
     <sheet name="ODR_INF" sheetId="18" r:id="rId2"/>
     <sheet name="ODR_INF_DETAIL" sheetId="19" r:id="rId3"/>
     <sheet name="TEN_MST" sheetId="22" r:id="rId4"/>
-    <sheet name="PT_SANTEI_CONF" sheetId="20" r:id="rId5"/>
-    <sheet name="USER_MST" sheetId="21" r:id="rId6"/>
-    <sheet name="TEKIOU_BYOMEI_MST" sheetId="23" r:id="rId7"/>
-    <sheet name="BYOMEI_MST" sheetId="24" r:id="rId8"/>
+    <sheet name="AUTO_SANTEI_MST" sheetId="25" r:id="rId5"/>
+    <sheet name="PT_SANTEI_CONF" sheetId="20" r:id="rId6"/>
+    <sheet name="USER_MST" sheetId="21" r:id="rId7"/>
+    <sheet name="TEKIOU_BYOMEI_MST" sheetId="23" r:id="rId8"/>
+    <sheet name="BYOMEI_MST" sheetId="24" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="318">
   <si>
     <t>HP_ID</t>
   </si>
@@ -953,6 +954,39 @@
   </si>
   <si>
     <t>Y90299</t>
+  </si>
+  <si>
+    <t>hp_id</t>
+  </si>
+  <si>
+    <t>item_cd</t>
+  </si>
+  <si>
+    <t>seq_no</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>create_date</t>
+  </si>
+  <si>
+    <t>create_id</t>
+  </si>
+  <si>
+    <t>create_machine</t>
+  </si>
+  <si>
+    <t>update_date</t>
+  </si>
+  <si>
+    <t>update_id</t>
+  </si>
+  <si>
+    <t>update_machine</t>
   </si>
 </sst>
 </file>
@@ -989,9 +1023,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2000,7 +2035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9146CE-ED57-41C2-9C61-24C07C4EF6D9}">
   <dimension ref="A1:GG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CX1" workbookViewId="0">
+    <sheetView topLeftCell="CX1" workbookViewId="0">
       <selection activeCell="DH8" sqref="DH8"/>
     </sheetView>
   </sheetViews>
@@ -3556,6 +3591,84 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{808E4163-D007-44EC-B63A-15DBB5CB6E6E}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I1" t="s">
+        <v>315</v>
+      </c>
+      <c r="J1" t="s">
+        <v>316</v>
+      </c>
+      <c r="K1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>111015970</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>99999999</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CEA432-92E2-43DD-9BF0-48A46549EDC6}">
   <dimension ref="A1:P3"/>
   <sheetViews>
@@ -3725,7 +3838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B31579-AACE-4522-97A1-65BE362EBAFC}">
   <dimension ref="A1:X2"/>
   <sheetViews>
@@ -3879,7 +3992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E2663C-D32A-45D5-BBD9-4224A7DC50B2}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -3997,7 +4110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9830985-1F87-4A2C-BCAE-09A96FE9D3D2}">
   <dimension ref="A1:AH2"/>
   <sheetViews>

</xml_diff>